<commit_message>
Did the Medium difficulty
</commit_message>
<xml_diff>
--- a/ExcelEsport/FMWC_Examples/Bear Island - Harry Seiders - with Answers.xlsx
+++ b/ExcelEsport/FMWC_Examples/Bear Island - Harry Seiders - with Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\ExcelEsport\FMWC_Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2688855E-76F1-4550-AC19-8C22852FCE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8310AC-01CA-41A9-8513-C32F3928BFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{114A3ACC-2F61-4F50-A5CF-63A86B2334B2}"/>
   </bookViews>
@@ -39,8 +39,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -51,16 +52,40 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="213">
   <si>
     <t>Bear Island</t>
   </si>
@@ -776,6 +801,12 @@
   <si>
     <t>Profit</t>
   </si>
+  <si>
+    <t>Bear Treat</t>
+  </si>
+  <si>
+    <t>Treat Value</t>
+  </si>
 </sst>
 </file>
 
@@ -963,7 +994,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1049,6 +1080,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF001838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1946,7 +1983,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2240,6 +2277,9 @@
     <xf numFmtId="0" fontId="14" fillId="11" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2336,9 +2376,7 @@
     <xf numFmtId="0" fontId="28" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2383,9 +2421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>247303</xdr:colOff>
+      <xdr:colOff>251113</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>324825</xdr:rowOff>
+      <xdr:rowOff>321015</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2429,7 +2467,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>1939652</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>359004</xdr:rowOff>
+      <xdr:rowOff>362814</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2590,6 +2628,72 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+  <rv s="1">
+    <v>13</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="propagated" t="b"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2891,8 +2995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1BDF3C-7CF1-4670-8742-2CB86BCAA1B5}">
   <dimension ref="A1:AV222"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N79" sqref="N79"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A101" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2911,7 +3015,8 @@
     <col min="12" max="12" width="7" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="32.21875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="4.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="28.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" style="1" customWidth="1"/>
     <col min="19" max="28" width="4.88671875" style="1" customWidth="1"/>
@@ -2948,19 +3053,19 @@
       <c r="AV1" s="4"/>
     </row>
     <row r="2" spans="2:48" ht="33.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
       <c r="N2" s="44" t="s">
         <v>1</v>
       </c>
@@ -3059,19 +3164,19 @@
       <c r="AV8" s="4"/>
     </row>
     <row r="9" spans="2:48" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="138"/>
-      <c r="K9" s="145" t="s">
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="139"/>
+      <c r="K9" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="145"/>
+      <c r="L9" s="146"/>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
@@ -3097,15 +3202,15 @@
       <c r="AV9" s="4"/>
     </row>
     <row r="10" spans="2:48" ht="14.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="127" t="s">
+      <c r="B10" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
+      <c r="H10" s="130"/>
       <c r="W10" s="20"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="20"/>
@@ -3132,13 +3237,13 @@
       <c r="AV10" s="4"/>
     </row>
     <row r="11" spans="2:48" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="130"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="132"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="132"/>
+      <c r="H11" s="133"/>
       <c r="K11" s="90" t="s">
         <v>6</v>
       </c>
@@ -3179,13 +3284,13 @@
       <c r="AV11" s="4"/>
     </row>
     <row r="12" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="131"/>
-      <c r="H12" s="132"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="132"/>
+      <c r="H12" s="133"/>
       <c r="K12" s="79" t="s">
         <v>7</v>
       </c>
@@ -3216,13 +3321,13 @@
       <c r="AV12" s="4"/>
     </row>
     <row r="13" spans="2:48" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="130"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="131"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="131"/>
-      <c r="H13" s="132"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="132"/>
+      <c r="H13" s="133"/>
       <c r="K13" s="58" t="s">
         <v>8</v>
       </c>
@@ -3263,13 +3368,13 @@
       <c r="AV13" s="4"/>
     </row>
     <row r="14" spans="2:48" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="130"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="131"/>
-      <c r="G14" s="131"/>
-      <c r="H14" s="132"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="133"/>
       <c r="K14" s="58" t="s">
         <v>9</v>
       </c>
@@ -3310,13 +3415,13 @@
       <c r="AV14" s="4"/>
     </row>
     <row r="15" spans="2:48" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="130"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="132"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="133"/>
       <c r="K15" s="58" t="s">
         <v>10</v>
       </c>
@@ -3350,13 +3455,13 @@
       <c r="AV15" s="4"/>
     </row>
     <row r="16" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="130"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="132"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="133"/>
       <c r="K16" s="58" t="s">
         <v>11</v>
       </c>
@@ -3390,13 +3495,13 @@
       <c r="AV16" s="4"/>
     </row>
     <row r="17" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="130"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="132"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="132"/>
+      <c r="H17" s="133"/>
       <c r="K17" s="58" t="s">
         <v>12</v>
       </c>
@@ -3427,13 +3532,13 @@
       <c r="AV17" s="4"/>
     </row>
     <row r="18" spans="2:48" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="133"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="135"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="136"/>
       <c r="K18" s="58" t="s">
         <v>13</v>
       </c>
@@ -3482,15 +3587,15 @@
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="2:48" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="126"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20" s="58" t="s">
@@ -3877,15 +3982,15 @@
       <c r="AV29" s="4"/>
     </row>
     <row r="30" spans="2:48" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="126" t="s">
+      <c r="B30" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="126"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="126"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="126"/>
-      <c r="H30" s="126"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
       <c r="I30" s="45"/>
       <c r="J30" s="45"/>
       <c r="K30" s="58" t="s">
@@ -4199,14 +4304,14 @@
       <c r="E41" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="G41" s="123" t="s">
+      <c r="G41" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="H41" s="124"/>
-      <c r="I41" s="124"/>
-      <c r="J41" s="124"/>
-      <c r="K41" s="124"/>
-      <c r="L41" s="125"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="125"/>
+      <c r="J41" s="125"/>
+      <c r="K41" s="125"/>
+      <c r="L41" s="126"/>
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
@@ -4242,14 +4347,18 @@
         <f>IF(ISBLANK(E42),0,IF(E42=Answers!E42,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G42" s="139" t="s">
+      <c r="G42" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="H42" s="140"/>
-      <c r="I42" s="140"/>
-      <c r="J42" s="140"/>
-      <c r="K42" s="140"/>
-      <c r="L42" s="141"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
+      <c r="J42" s="141"/>
+      <c r="K42" s="141"/>
+      <c r="L42" s="142"/>
+      <c r="N42" s="1" t="b" cm="1">
+        <f t="array" ref="N42:N44">D33:D35=I113</f>
+        <v>1</v>
+      </c>
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
@@ -4285,14 +4394,17 @@
         <f>IF(ISBLANK(E43),0,IF(E43=Answers!E43,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G43" s="142" t="s">
+      <c r="G43" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="H43" s="143"/>
-      <c r="I43" s="143"/>
-      <c r="J43" s="143"/>
-      <c r="K43" s="143"/>
-      <c r="L43" s="144"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="144"/>
+      <c r="J43" s="144"/>
+      <c r="K43" s="144"/>
+      <c r="L43" s="145"/>
+      <c r="N43" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
       <c r="AF43" s="4"/>
@@ -4328,14 +4440,17 @@
         <f>IF(ISBLANK(E44),0,IF(E44=Answers!E44,1,-1))</f>
         <v>0</v>
       </c>
-      <c r="G44" s="120" t="s">
+      <c r="G44" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121"/>
-      <c r="J44" s="121"/>
-      <c r="K44" s="121"/>
-      <c r="L44" s="122"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="122"/>
+      <c r="J44" s="122"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="123"/>
+      <c r="N44" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
       <c r="AF44" s="4"/>
@@ -4467,9 +4582,9 @@
       <c r="AV49" s="4"/>
     </row>
     <row r="50" spans="2:48" ht="14.85" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="K50" s="117">
+      <c r="K50" s="118">
         <f>SUMPRODUCT(D:D,F:F)</f>
-        <v>220</v>
+        <v>420</v>
       </c>
       <c r="AK50" s="4"/>
       <c r="AL50" s="4"/>
@@ -4488,7 +4603,7 @@
       <c r="B51" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="K51" s="118"/>
+      <c r="K51" s="119"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="AK51" s="4"/>
@@ -4507,7 +4622,7 @@
     <row r="52" spans="2:48" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="22"/>
       <c r="G52" s="26"/>
-      <c r="K52" s="118"/>
+      <c r="K52" s="119"/>
       <c r="P52" s="4"/>
       <c r="Q52" s="4"/>
       <c r="AK52" s="4"/>
@@ -4542,7 +4657,7 @@
       <c r="H53" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="K53" s="119"/>
+      <c r="K53" s="120"/>
       <c r="P53" s="4"/>
       <c r="Q53" s="4"/>
       <c r="AK53" s="4"/>
@@ -4667,7 +4782,7 @@
         <f>IF(ISBLANK(E57),0,IF(E57=Answers!E57,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G57" s="147" t="s">
+      <c r="G57" s="115" t="s">
         <v>22</v>
       </c>
       <c r="H57" s="25">
@@ -4719,7 +4834,7 @@
         <f>IF(ISBLANK(E58),0,IF(E58=Answers!E58,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G58" s="147" t="s">
+      <c r="G58" s="115" t="s">
         <v>31</v>
       </c>
       <c r="H58" s="25">
@@ -4770,7 +4885,7 @@
         <f>IF(ISBLANK(E59),0,IF(E59=Answers!E59,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G59" s="147" t="s">
+      <c r="G59" s="115" t="s">
         <v>34</v>
       </c>
       <c r="H59" s="25">
@@ -4821,7 +4936,7 @@
         <f>IF(ISBLANK(E60),0,IF(E60=Answers!E60,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G60" s="147" t="s">
+      <c r="G60" s="115" t="s">
         <v>82</v>
       </c>
       <c r="H60" s="25">
@@ -4872,7 +4987,7 @@
         <f>IF(ISBLANK(E61),0,IF(E61=Answers!E61,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G61" s="147" t="s">
+      <c r="G61" s="115" t="s">
         <v>28</v>
       </c>
       <c r="H61" s="25">
@@ -4923,7 +5038,7 @@
         <f>IF(ISBLANK(E62),0,IF(E62=Answers!E62,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G62" s="147" t="s">
+      <c r="G62" s="115" t="s">
         <v>83</v>
       </c>
       <c r="H62" s="25">
@@ -4975,7 +5090,7 @@
         <f>IF(ISBLANK(E63),0,IF(E63=Answers!E63,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G63" s="147" t="s">
+      <c r="G63" s="115" t="s">
         <v>34</v>
       </c>
       <c r="H63" s="25">
@@ -5026,7 +5141,7 @@
         <f>IF(ISBLANK(E64),0,IF(E64=Answers!E64,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G64" s="147" t="s">
+      <c r="G64" s="115" t="s">
         <v>37</v>
       </c>
       <c r="H64" s="25">
@@ -5077,7 +5192,7 @@
         <f>IF(ISBLANK(E65),0,IF(E65=Answers!E65,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G65" s="147" t="s">
+      <c r="G65" s="115" t="s">
         <v>84</v>
       </c>
       <c r="H65" s="25">
@@ -5128,7 +5243,7 @@
         <f>IF(ISBLANK(E66),0,IF(E66=Answers!E66,1,-1))</f>
         <v>1</v>
       </c>
-      <c r="G66" s="147" t="s">
+      <c r="G66" s="115" t="s">
         <v>83</v>
       </c>
       <c r="H66" s="25">
@@ -5488,7 +5603,7 @@
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="J80" s="1" t="e">
-        <f t="shared" ref="J80:J100" si="6">H80*_xlfn.XLOOKUP(G80,$N$56:$N$66,$O$56:$O$66)</f>
+        <f t="shared" ref="J80" si="6">H80*_xlfn.XLOOKUP(G80,$N$56:$N$66,$O$56:$O$66)</f>
         <v>#N/A</v>
       </c>
       <c r="K80" s="1" t="e">
@@ -6768,6 +6883,18 @@
       <c r="I111" s="60" t="s">
         <v>98</v>
       </c>
+      <c r="K111" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N111" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AB111" s="4"/>
       <c r="AC111" s="4"/>
       <c r="AD111" s="4"/>
@@ -6843,6 +6970,25 @@
       <c r="I113" s="25" t="s">
         <v>50</v>
       </c>
+      <c r="J113" s="148"/>
+      <c r="K113" s="148">
+        <f>H113*_xlfn.XLOOKUP(G113,$N$56:$N$67,$O$56:$O$67)</f>
+        <v>600</v>
+      </c>
+      <c r="L113" s="148"/>
+      <c r="M113" s="148">
+        <f>H113*_xlfn.XLOOKUP(G113,$Q$23:$Q$34,$O$23:$O$34)</f>
+        <v>450</v>
+      </c>
+      <c r="N113" s="148" t="str" cm="1">
+        <f t="array" ref="N113">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I113))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="O113" s="148"/>
+      <c r="P113" s="148">
+        <f>H113*_xlfn.XLOOKUP(N113,$K$12:$K$36,$L$12:$L$36)</f>
+        <v>36</v>
+      </c>
       <c r="AB113" s="4"/>
       <c r="AC113" s="4"/>
       <c r="AD113" s="4"/>
@@ -6870,6 +7016,18 @@
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
+      <c r="K114" s="148" t="e">
+        <f t="shared" ref="K114:K134" si="10">H114*_xlfn.XLOOKUP(G114,$N$56:$N$67,$O$56:$O$67)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N114" s="148" t="e" cm="1" vm="1">
+        <f t="array" ref="N114">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I114))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P114" s="148" t="e" vm="2">
+        <f t="shared" ref="P114:P135" si="11">H114*_xlfn.XLOOKUP(N114,$K$12:$K$36,$L$12:$L$36)</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="AB114" s="4"/>
       <c r="AC114" s="4"/>
       <c r="AD114" s="4"/>
@@ -6902,10 +7060,13 @@
       <c r="D115" s="18">
         <v>10</v>
       </c>
-      <c r="E115" s="19"/>
+      <c r="E115" s="19">
+        <f t="shared" ref="E115:E119" si="12">K115-P115</f>
+        <v>1088</v>
+      </c>
       <c r="F115" s="37">
         <f>IF(ISBLANK(E115),0,IF(E115=Answers!E115,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115" s="25" t="s">
         <v>22</v>
@@ -6915,6 +7076,18 @@
       </c>
       <c r="I115" s="25" t="s">
         <v>56</v>
+      </c>
+      <c r="K115" s="148">
+        <f t="shared" si="10"/>
+        <v>1120</v>
+      </c>
+      <c r="N115" s="148" t="str" cm="1">
+        <f t="array" ref="N115">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I115))</f>
+        <v>Raspberries</v>
+      </c>
+      <c r="P115" s="148">
+        <f t="shared" si="11"/>
+        <v>32</v>
       </c>
       <c r="AB115" s="4"/>
       <c r="AC115" s="4"/>
@@ -6949,10 +7122,13 @@
       <c r="D116" s="18">
         <v>10</v>
       </c>
-      <c r="E116" s="19"/>
+      <c r="E116" s="19">
+        <f t="shared" si="12"/>
+        <v>459</v>
+      </c>
       <c r="F116" s="37">
         <f>IF(ISBLANK(E116),0,IF(E116=Answers!E116,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116" s="25" t="s">
         <v>31</v>
@@ -6962,6 +7138,18 @@
       </c>
       <c r="I116" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K116" s="148">
+        <f t="shared" si="10"/>
+        <v>480</v>
+      </c>
+      <c r="N116" s="148" t="str" cm="1">
+        <f t="array" ref="N116">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I116))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P116" s="148">
+        <f t="shared" si="11"/>
+        <v>21</v>
       </c>
       <c r="AB116" s="4"/>
       <c r="AC116" s="4"/>
@@ -6996,10 +7184,13 @@
       <c r="D117" s="18">
         <v>10</v>
       </c>
-      <c r="E117" s="19"/>
+      <c r="E117" s="19">
+        <f t="shared" si="12"/>
+        <v>1862</v>
+      </c>
       <c r="F117" s="37">
         <f>IF(ISBLANK(E117),0,IF(E117=Answers!E117,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117" s="25" t="s">
         <v>34</v>
@@ -7009,6 +7200,18 @@
       </c>
       <c r="I117" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K117" s="148">
+        <f t="shared" si="10"/>
+        <v>2030</v>
+      </c>
+      <c r="N117" s="148" t="str" cm="1">
+        <f t="array" ref="N117">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I117))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P117" s="148">
+        <f>H117*_xlfn.XLOOKUP(N117,$K$12:$K$36,$L$12:$L$36)</f>
+        <v>168</v>
       </c>
       <c r="AB117" s="4"/>
       <c r="AC117" s="4"/>
@@ -7043,10 +7246,13 @@
       <c r="D118" s="18">
         <v>10</v>
       </c>
-      <c r="E118" s="19"/>
+      <c r="E118" s="19">
+        <f t="shared" si="12"/>
+        <v>1188</v>
+      </c>
       <c r="F118" s="37">
         <f>IF(ISBLANK(E118),0,IF(E118=Answers!E118,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G118" s="25" t="s">
         <v>82</v>
@@ -7056,6 +7262,18 @@
       </c>
       <c r="I118" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K118" s="148">
+        <f t="shared" si="10"/>
+        <v>1260</v>
+      </c>
+      <c r="N118" s="148" t="str" cm="1">
+        <f t="array" ref="N118">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I118))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P118" s="148">
+        <f t="shared" si="11"/>
+        <v>72</v>
       </c>
       <c r="AB118" s="4"/>
       <c r="AC118" s="4"/>
@@ -7090,10 +7308,13 @@
       <c r="D119" s="18">
         <v>10</v>
       </c>
-      <c r="E119" s="19"/>
+      <c r="E119" s="19">
+        <f t="shared" si="12"/>
+        <v>1057</v>
+      </c>
       <c r="F119" s="37">
         <f>IF(ISBLANK(E119),0,IF(E119=Answers!E119,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119" s="25" t="s">
         <v>28</v>
@@ -7103,6 +7324,18 @@
       </c>
       <c r="I119" s="25" t="s">
         <v>56</v>
+      </c>
+      <c r="K119" s="148">
+        <f t="shared" si="10"/>
+        <v>1085</v>
+      </c>
+      <c r="N119" s="148" t="str" cm="1">
+        <f t="array" ref="N119">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I119))</f>
+        <v>Raspberries</v>
+      </c>
+      <c r="P119" s="148">
+        <f t="shared" si="11"/>
+        <v>28</v>
       </c>
       <c r="AB119" s="4"/>
       <c r="AC119" s="4"/>
@@ -7137,10 +7370,13 @@
       <c r="D120" s="18">
         <v>10</v>
       </c>
-      <c r="E120" s="19"/>
+      <c r="E120" s="19">
+        <f t="shared" ref="E120:E133" si="13">K120-P120</f>
+        <v>1464</v>
+      </c>
       <c r="F120" s="37">
         <f>IF(ISBLANK(E120),0,IF(E120=Answers!E120,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120" s="25" t="s">
         <v>83</v>
@@ -7150,6 +7386,18 @@
       </c>
       <c r="I120" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K120" s="148">
+        <f t="shared" si="10"/>
+        <v>1520</v>
+      </c>
+      <c r="N120" s="148" t="str" cm="1">
+        <f t="array" ref="N120">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I120))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P120" s="148">
+        <f t="shared" si="11"/>
+        <v>56</v>
       </c>
       <c r="AB120" s="4"/>
       <c r="AC120" s="4"/>
@@ -7184,10 +7432,13 @@
       <c r="D121" s="18">
         <v>10</v>
       </c>
-      <c r="E121" s="19"/>
+      <c r="E121" s="19">
+        <f t="shared" si="13"/>
+        <v>931</v>
+      </c>
       <c r="F121" s="37">
         <f>IF(ISBLANK(E121),0,IF(E121=Answers!E121,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121" s="25" t="s">
         <v>34</v>
@@ -7197,6 +7448,18 @@
       </c>
       <c r="I121" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K121" s="148">
+        <f t="shared" si="10"/>
+        <v>1015</v>
+      </c>
+      <c r="N121" s="148" t="str" cm="1">
+        <f t="array" ref="N121">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I121))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P121" s="148">
+        <f t="shared" si="11"/>
+        <v>84</v>
       </c>
       <c r="AB121" s="4"/>
       <c r="AC121" s="4"/>
@@ -7231,10 +7494,13 @@
       <c r="D122" s="18">
         <v>10</v>
       </c>
-      <c r="E122" s="19"/>
+      <c r="E122" s="19">
+        <f t="shared" si="13"/>
+        <v>1422</v>
+      </c>
       <c r="F122" s="37">
         <f>IF(ISBLANK(E122),0,IF(E122=Answers!E122,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122" s="25" t="s">
         <v>37</v>
@@ -7244,6 +7510,18 @@
       </c>
       <c r="I122" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K122" s="148">
+        <f t="shared" si="10"/>
+        <v>1530</v>
+      </c>
+      <c r="N122" s="148" t="str" cm="1">
+        <f t="array" ref="N122">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I122))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P122" s="148">
+        <f t="shared" si="11"/>
+        <v>108</v>
       </c>
       <c r="AB122" s="4"/>
       <c r="AC122" s="4"/>
@@ -7269,7 +7547,7 @@
     </row>
     <row r="123" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B123" s="17">
-        <f t="shared" ref="B123:B188" si="10">B122+1</f>
+        <f t="shared" ref="B123:B188" si="14">B122+1</f>
         <v>39</v>
       </c>
       <c r="C123" s="17">
@@ -7278,10 +7556,13 @@
       <c r="D123" s="18">
         <v>10</v>
       </c>
-      <c r="E123" s="19"/>
+      <c r="E123" s="19">
+        <f t="shared" si="13"/>
+        <v>1692</v>
+      </c>
       <c r="F123" s="37">
         <f>IF(ISBLANK(E123),0,IF(E123=Answers!E123,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G123" s="25" t="s">
         <v>84</v>
@@ -7291,6 +7572,18 @@
       </c>
       <c r="I123" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K123" s="148">
+        <f t="shared" si="10"/>
+        <v>1755</v>
+      </c>
+      <c r="N123" s="148" t="str" cm="1">
+        <f t="array" ref="N123">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I123))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P123" s="148">
+        <f t="shared" si="11"/>
+        <v>63</v>
       </c>
       <c r="AB123" s="4"/>
       <c r="AC123" s="4"/>
@@ -7316,7 +7609,7 @@
     </row>
     <row r="124" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B124" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>40</v>
       </c>
       <c r="C124" s="17">
@@ -7325,10 +7618,13 @@
       <c r="D124" s="18">
         <v>10</v>
       </c>
-      <c r="E124" s="19"/>
+      <c r="E124" s="19">
+        <f t="shared" si="13"/>
+        <v>1302</v>
+      </c>
       <c r="F124" s="37">
         <f>IF(ISBLANK(E124),0,IF(E124=Answers!E124,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G124" s="25" t="s">
         <v>83</v>
@@ -7338,6 +7634,18 @@
       </c>
       <c r="I124" s="25" t="s">
         <v>56</v>
+      </c>
+      <c r="K124" s="148">
+        <f t="shared" si="10"/>
+        <v>1330</v>
+      </c>
+      <c r="N124" s="148" t="str" cm="1">
+        <f t="array" ref="N124">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I124))</f>
+        <v>Raspberries</v>
+      </c>
+      <c r="P124" s="148">
+        <f t="shared" si="11"/>
+        <v>28</v>
       </c>
       <c r="AB124" s="4"/>
       <c r="AC124" s="4"/>
@@ -7363,7 +7671,7 @@
     </row>
     <row r="125" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B125" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>41</v>
       </c>
       <c r="C125" s="17">
@@ -7372,10 +7680,13 @@
       <c r="D125" s="18">
         <v>10</v>
       </c>
-      <c r="E125" s="19"/>
+      <c r="E125" s="19">
+        <f t="shared" si="13"/>
+        <v>2013</v>
+      </c>
       <c r="F125" s="37">
         <f>IF(ISBLANK(E125),0,IF(E125=Answers!E125,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" s="25" t="s">
         <v>84</v>
@@ -7385,6 +7696,18 @@
       </c>
       <c r="I125" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K125" s="148">
+        <f t="shared" si="10"/>
+        <v>2145</v>
+      </c>
+      <c r="N125" s="148" t="str" cm="1">
+        <f t="array" ref="N125">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I125))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P125" s="148">
+        <f t="shared" si="11"/>
+        <v>132</v>
       </c>
       <c r="AB125" s="4"/>
       <c r="AC125" s="4"/>
@@ -7410,7 +7733,7 @@
     </row>
     <row r="126" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B126" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>42</v>
       </c>
       <c r="C126" s="17">
@@ -7419,10 +7742,13 @@
       <c r="D126" s="18">
         <v>10</v>
       </c>
-      <c r="E126" s="19"/>
+      <c r="E126" s="19">
+        <f t="shared" si="13"/>
+        <v>2976</v>
+      </c>
       <c r="F126" s="37">
         <f>IF(ISBLANK(E126),0,IF(E126=Answers!E126,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" s="25" t="s">
         <v>83</v>
@@ -7432,6 +7758,18 @@
       </c>
       <c r="I126" s="25" t="s">
         <v>56</v>
+      </c>
+      <c r="K126" s="148">
+        <f t="shared" si="10"/>
+        <v>3040</v>
+      </c>
+      <c r="N126" s="148" t="str" cm="1">
+        <f t="array" ref="N126">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I126))</f>
+        <v>Raspberries</v>
+      </c>
+      <c r="P126" s="148">
+        <f t="shared" si="11"/>
+        <v>64</v>
       </c>
       <c r="AB126" s="4"/>
       <c r="AC126" s="4"/>
@@ -7457,7 +7795,7 @@
     </row>
     <row r="127" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B127" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>43</v>
       </c>
       <c r="C127" s="17">
@@ -7466,10 +7804,13 @@
       <c r="D127" s="18">
         <v>10</v>
       </c>
-      <c r="E127" s="19"/>
+      <c r="E127" s="19">
+        <f t="shared" si="13"/>
+        <v>2249</v>
+      </c>
       <c r="F127" s="37">
         <f>IF(ISBLANK(E127),0,IF(E127=Answers!E127,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G127" s="25" t="s">
         <v>92</v>
@@ -7479,6 +7820,18 @@
       </c>
       <c r="I127" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K127" s="148">
+        <f t="shared" si="10"/>
+        <v>2340</v>
+      </c>
+      <c r="N127" s="148" t="str" cm="1">
+        <f t="array" ref="N127">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I127))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P127" s="148">
+        <f t="shared" si="11"/>
+        <v>91</v>
       </c>
       <c r="AB127" s="4"/>
       <c r="AC127" s="4"/>
@@ -7504,7 +7857,7 @@
     </row>
     <row r="128" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B128" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>44</v>
       </c>
       <c r="C128" s="17">
@@ -7513,10 +7866,13 @@
       <c r="D128" s="18">
         <v>10</v>
       </c>
-      <c r="E128" s="19"/>
+      <c r="E128" s="19">
+        <f t="shared" si="13"/>
+        <v>4116</v>
+      </c>
       <c r="F128" s="37">
         <f>IF(ISBLANK(E128),0,IF(E128=Answers!E128,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G128" s="25" t="s">
         <v>81</v>
@@ -7526,6 +7882,18 @@
       </c>
       <c r="I128" s="25" t="s">
         <v>56</v>
+      </c>
+      <c r="K128" s="148">
+        <f t="shared" si="10"/>
+        <v>4200</v>
+      </c>
+      <c r="N128" s="148" t="str" cm="1">
+        <f t="array" ref="N128">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I128))</f>
+        <v>Raspberries</v>
+      </c>
+      <c r="P128" s="148">
+        <f t="shared" si="11"/>
+        <v>84</v>
       </c>
       <c r="AB128" s="4"/>
       <c r="AC128" s="4"/>
@@ -7551,7 +7919,7 @@
     </row>
     <row r="129" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B129" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>45</v>
       </c>
       <c r="C129" s="17">
@@ -7560,10 +7928,13 @@
       <c r="D129" s="18">
         <v>10</v>
       </c>
-      <c r="E129" s="19"/>
+      <c r="E129" s="19">
+        <f t="shared" si="13"/>
+        <v>2670</v>
+      </c>
       <c r="F129" s="37">
         <f>IF(ISBLANK(E129),0,IF(E129=Answers!E129,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G129" s="25" t="s">
         <v>93</v>
@@ -7573,6 +7944,18 @@
       </c>
       <c r="I129" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K129" s="148">
+        <f t="shared" si="10"/>
+        <v>2775</v>
+      </c>
+      <c r="N129" s="148" t="str" cm="1">
+        <f t="array" ref="N129">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I129))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P129" s="148">
+        <f t="shared" si="11"/>
+        <v>105</v>
       </c>
       <c r="AB129" s="4"/>
       <c r="AC129" s="4"/>
@@ -7598,7 +7981,7 @@
     </row>
     <row r="130" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B130" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>46</v>
       </c>
       <c r="C130" s="17">
@@ -7607,10 +7990,13 @@
       <c r="D130" s="18">
         <v>10</v>
       </c>
-      <c r="E130" s="19"/>
+      <c r="E130" s="19">
+        <f t="shared" si="13"/>
+        <v>752</v>
+      </c>
       <c r="F130" s="37">
         <f>IF(ISBLANK(E130),0,IF(E130=Answers!E130,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G130" s="25" t="s">
         <v>84</v>
@@ -7620,6 +8006,18 @@
       </c>
       <c r="I130" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K130" s="148">
+        <f t="shared" si="10"/>
+        <v>780</v>
+      </c>
+      <c r="N130" s="148" t="str" cm="1">
+        <f t="array" ref="N130">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I130))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P130" s="148">
+        <f t="shared" si="11"/>
+        <v>28</v>
       </c>
       <c r="AB130" s="4"/>
       <c r="AC130" s="4"/>
@@ -7645,7 +8043,7 @@
     </row>
     <row r="131" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B131" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>47</v>
       </c>
       <c r="C131" s="17">
@@ -7654,10 +8052,13 @@
       <c r="D131" s="18">
         <v>10</v>
       </c>
-      <c r="E131" s="19"/>
+      <c r="E131" s="19">
+        <f t="shared" si="13"/>
+        <v>865</v>
+      </c>
       <c r="F131" s="37">
         <f>IF(ISBLANK(E131),0,IF(E131=Answers!E131,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G131" s="25" t="s">
         <v>93</v>
@@ -7667,6 +8068,18 @@
       </c>
       <c r="I131" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K131" s="148">
+        <f t="shared" si="10"/>
+        <v>925</v>
+      </c>
+      <c r="N131" s="148" t="str" cm="1">
+        <f t="array" ref="N131">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I131))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P131" s="148">
+        <f t="shared" si="11"/>
+        <v>60</v>
       </c>
       <c r="AB131" s="4"/>
       <c r="AC131" s="4"/>
@@ -7692,7 +8105,7 @@
     </row>
     <row r="132" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B132" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>48</v>
       </c>
       <c r="C132" s="17">
@@ -7701,10 +8114,13 @@
       <c r="D132" s="18">
         <v>10</v>
       </c>
-      <c r="E132" s="19"/>
+      <c r="E132" s="19">
+        <f t="shared" si="13"/>
+        <v>2907</v>
+      </c>
       <c r="F132" s="37">
         <f>IF(ISBLANK(E132),0,IF(E132=Answers!E132,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G132" s="25" t="s">
         <v>31</v>
@@ -7714,6 +8130,18 @@
       </c>
       <c r="I132" s="25" t="s">
         <v>53</v>
+      </c>
+      <c r="K132" s="148">
+        <f t="shared" si="10"/>
+        <v>3040</v>
+      </c>
+      <c r="N132" s="148" t="str" cm="1">
+        <f t="array" ref="N132">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I132))</f>
+        <v>Bamboo</v>
+      </c>
+      <c r="P132" s="148">
+        <f t="shared" si="11"/>
+        <v>133</v>
       </c>
       <c r="AB132" s="4"/>
       <c r="AC132" s="4"/>
@@ -7739,7 +8167,7 @@
     </row>
     <row r="133" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B133" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>49</v>
       </c>
       <c r="C133" s="17">
@@ -7748,10 +8176,13 @@
       <c r="D133" s="18">
         <v>10</v>
       </c>
-      <c r="E133" s="19"/>
+      <c r="E133" s="19">
+        <f t="shared" si="13"/>
+        <v>1833</v>
+      </c>
       <c r="F133" s="37">
         <f>IF(ISBLANK(E133),0,IF(E133=Answers!E133,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133" s="25" t="s">
         <v>34</v>
@@ -7761,6 +8192,18 @@
       </c>
       <c r="I133" s="25" t="s">
         <v>56</v>
+      </c>
+      <c r="K133" s="148">
+        <f t="shared" si="10"/>
+        <v>1885</v>
+      </c>
+      <c r="N133" s="148" t="str" cm="1">
+        <f t="array" ref="N133">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I133))</f>
+        <v>Raspberries</v>
+      </c>
+      <c r="P133" s="148">
+        <f t="shared" si="11"/>
+        <v>52</v>
       </c>
       <c r="AB133" s="4"/>
       <c r="AC133" s="4"/>
@@ -7786,7 +8229,7 @@
     </row>
     <row r="134" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B134" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>50</v>
       </c>
       <c r="C134" s="17">
@@ -7795,10 +8238,13 @@
       <c r="D134" s="18">
         <v>10</v>
       </c>
-      <c r="E134" s="19"/>
+      <c r="E134" s="19">
+        <f>K134-P134</f>
+        <v>2686</v>
+      </c>
       <c r="F134" s="37">
         <f>IF(ISBLANK(E134),0,IF(E134=Answers!E134,1,-1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G134" s="25" t="s">
         <v>37</v>
@@ -7808,6 +8254,18 @@
       </c>
       <c r="I134" s="25" t="s">
         <v>50</v>
+      </c>
+      <c r="K134" s="148">
+        <f t="shared" si="10"/>
+        <v>2890</v>
+      </c>
+      <c r="N134" s="148" t="str" cm="1">
+        <f t="array" ref="N134">_xlfn._xlws.FILTER($F$33:$F$35,--($D$33:$D$35=I134))</f>
+        <v>Eucalyptus</v>
+      </c>
+      <c r="P134" s="148">
+        <f t="shared" si="11"/>
+        <v>204</v>
       </c>
       <c r="AB134" s="4"/>
       <c r="AC134" s="4"/>
@@ -7837,6 +8295,7 @@
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="5"/>
+      <c r="P135" s="148"/>
       <c r="AK135" s="4"/>
       <c r="AL135" s="4"/>
       <c r="AM135" s="4"/>
@@ -7862,11 +8321,11 @@
       </c>
       <c r="E136" s="19">
         <f>SUM(E115:E134)</f>
-        <v>0</v>
+        <v>35532</v>
       </c>
       <c r="F136" s="37">
         <f>IF(ISBLANK(E136),0,IF(E136=Answers!E136,1,-1))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AK136" s="4"/>
       <c r="AL136" s="4"/>
@@ -8209,7 +8668,7 @@
     </row>
     <row r="150" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B150" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>52</v>
       </c>
       <c r="C150" s="17">
@@ -8247,7 +8706,7 @@
     </row>
     <row r="151" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B151" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>53</v>
       </c>
       <c r="C151" s="17">
@@ -8285,7 +8744,7 @@
     </row>
     <row r="152" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B152" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>54</v>
       </c>
       <c r="C152" s="17">
@@ -8323,7 +8782,7 @@
     </row>
     <row r="153" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B153" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>55</v>
       </c>
       <c r="C153" s="17">
@@ -8361,7 +8820,7 @@
     </row>
     <row r="154" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B154" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>56</v>
       </c>
       <c r="C154" s="17">
@@ -8399,7 +8858,7 @@
     </row>
     <row r="155" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B155" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>57</v>
       </c>
       <c r="C155" s="17">
@@ -8437,7 +8896,7 @@
     </row>
     <row r="156" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B156" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>58</v>
       </c>
       <c r="C156" s="17">
@@ -8475,7 +8934,7 @@
     </row>
     <row r="157" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B157" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>59</v>
       </c>
       <c r="C157" s="17">
@@ -8513,7 +8972,7 @@
     </row>
     <row r="158" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B158" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>60</v>
       </c>
       <c r="C158" s="17">
@@ -8551,7 +9010,7 @@
     </row>
     <row r="159" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B159" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>61</v>
       </c>
       <c r="C159" s="17">
@@ -8589,7 +9048,7 @@
     </row>
     <row r="160" spans="2:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B160" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>62</v>
       </c>
       <c r="C160" s="17">
@@ -8627,7 +9086,7 @@
     </row>
     <row r="161" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B161" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>63</v>
       </c>
       <c r="C161" s="17">
@@ -8665,7 +9124,7 @@
     </row>
     <row r="162" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B162" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>64</v>
       </c>
       <c r="C162" s="17">
@@ -8703,7 +9162,7 @@
     </row>
     <row r="163" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B163" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>65</v>
       </c>
       <c r="C163" s="17">
@@ -8741,7 +9200,7 @@
     </row>
     <row r="164" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B164" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>66</v>
       </c>
       <c r="C164" s="17">
@@ -8779,7 +9238,7 @@
     </row>
     <row r="165" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="B165" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>67</v>
       </c>
       <c r="C165" s="17">
@@ -8817,7 +9276,7 @@
     </row>
     <row r="166" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B166" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>68</v>
       </c>
       <c r="C166" s="17">
@@ -8855,7 +9314,7 @@
     </row>
     <row r="167" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B167" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>69</v>
       </c>
       <c r="C167" s="17">
@@ -8893,7 +9352,7 @@
     </row>
     <row r="168" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B168" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>70</v>
       </c>
       <c r="C168" s="17">
@@ -9751,7 +10210,7 @@
     </row>
     <row r="185" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B185" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>72</v>
       </c>
       <c r="C185" s="17">
@@ -9812,7 +10271,7 @@
     </row>
     <row r="186" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B186" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>73</v>
       </c>
       <c r="C186" s="17">
@@ -9873,7 +10332,7 @@
     </row>
     <row r="187" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B187" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>74</v>
       </c>
       <c r="C187" s="17">
@@ -9934,7 +10393,7 @@
     </row>
     <row r="188" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B188" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>75</v>
       </c>
       <c r="C188" s="17">
@@ -9995,7 +10454,7 @@
     </row>
     <row r="189" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B189" s="17">
-        <f t="shared" ref="B189:B213" si="11">B188+1</f>
+        <f t="shared" ref="B189:B213" si="15">B188+1</f>
         <v>76</v>
       </c>
       <c r="C189" s="17">
@@ -10056,7 +10515,7 @@
     </row>
     <row r="190" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B190" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>77</v>
       </c>
       <c r="C190" s="17">
@@ -10117,7 +10576,7 @@
     </row>
     <row r="191" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B191" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>78</v>
       </c>
       <c r="C191" s="17">
@@ -10178,7 +10637,7 @@
     </row>
     <row r="192" spans="1:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B192" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>79</v>
       </c>
       <c r="C192" s="17">
@@ -10239,7 +10698,7 @@
     </row>
     <row r="193" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B193" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>80</v>
       </c>
       <c r="C193" s="17">
@@ -10300,7 +10759,7 @@
     </row>
     <row r="194" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B194" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>81</v>
       </c>
       <c r="C194" s="17">
@@ -10361,7 +10820,7 @@
     </row>
     <row r="195" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B195" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>82</v>
       </c>
       <c r="C195" s="17">
@@ -10422,7 +10881,7 @@
     </row>
     <row r="196" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B196" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>83</v>
       </c>
       <c r="C196" s="17">
@@ -10483,7 +10942,7 @@
     </row>
     <row r="197" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B197" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>84</v>
       </c>
       <c r="C197" s="17">
@@ -10544,7 +11003,7 @@
     </row>
     <row r="198" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B198" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>85</v>
       </c>
       <c r="C198" s="17">
@@ -10605,7 +11064,7 @@
     </row>
     <row r="199" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B199" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>86</v>
       </c>
       <c r="C199" s="17">
@@ -10666,7 +11125,7 @@
     </row>
     <row r="200" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B200" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>87</v>
       </c>
       <c r="C200" s="17">
@@ -10727,7 +11186,7 @@
     </row>
     <row r="201" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B201" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>88</v>
       </c>
       <c r="C201" s="17">
@@ -10788,7 +11247,7 @@
     </row>
     <row r="202" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B202" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>89</v>
       </c>
       <c r="C202" s="17">
@@ -10849,7 +11308,7 @@
     </row>
     <row r="203" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B203" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>90</v>
       </c>
       <c r="C203" s="17">
@@ -10910,7 +11369,7 @@
     </row>
     <row r="204" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B204" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>91</v>
       </c>
       <c r="C204" s="17">
@@ -10971,7 +11430,7 @@
     </row>
     <row r="205" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B205" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>92</v>
       </c>
       <c r="C205" s="17">
@@ -11032,7 +11491,7 @@
     </row>
     <row r="206" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B206" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>93</v>
       </c>
       <c r="C206" s="17">
@@ -11093,7 +11552,7 @@
     </row>
     <row r="207" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B207" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>94</v>
       </c>
       <c r="C207" s="17">
@@ -11154,7 +11613,7 @@
     </row>
     <row r="208" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B208" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>95</v>
       </c>
       <c r="C208" s="17">
@@ -11215,7 +11674,7 @@
     </row>
     <row r="209" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B209" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>96</v>
       </c>
       <c r="C209" s="17">
@@ -11276,7 +11735,7 @@
     </row>
     <row r="210" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B210" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>97</v>
       </c>
       <c r="C210" s="17">
@@ -11337,7 +11796,7 @@
     </row>
     <row r="211" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B211" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>98</v>
       </c>
       <c r="C211" s="17">
@@ -11398,7 +11857,7 @@
     </row>
     <row r="212" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B212" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>99</v>
       </c>
       <c r="C212" s="17">
@@ -11459,7 +11918,7 @@
     </row>
     <row r="213" spans="2:48" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B213" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="C213" s="17">
@@ -12007,19 +12466,19 @@
       <c r="AV1" s="4"/>
     </row>
     <row r="2" spans="2:48" ht="33.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
       <c r="N2" s="44" t="s">
         <v>1</v>
       </c>
@@ -12118,19 +12577,19 @@
       <c r="AV8" s="4"/>
     </row>
     <row r="9" spans="2:48" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="136" t="s">
+      <c r="B9" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="137"/>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="138"/>
-      <c r="K9" s="145" t="s">
+      <c r="C9" s="138"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="139"/>
+      <c r="K9" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="145"/>
+      <c r="L9" s="146"/>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
@@ -12156,15 +12615,15 @@
       <c r="AV9" s="4"/>
     </row>
     <row r="10" spans="2:48" ht="14.85" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="146" t="s">
+      <c r="B10" s="147" t="s">
         <v>206</v>
       </c>
-      <c r="C10" s="128"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="128"/>
-      <c r="H10" s="129"/>
+      <c r="C10" s="129"/>
+      <c r="D10" s="129"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
+      <c r="G10" s="129"/>
+      <c r="H10" s="130"/>
       <c r="W10" s="20"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="20"/>
@@ -12191,13 +12650,13 @@
       <c r="AV10" s="4"/>
     </row>
     <row r="11" spans="2:48" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="130"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="132"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="132"/>
+      <c r="H11" s="133"/>
       <c r="K11" s="90" t="s">
         <v>6</v>
       </c>
@@ -12231,13 +12690,13 @@
       <c r="AV11" s="4"/>
     </row>
     <row r="12" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="131"/>
-      <c r="H12" s="132"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="132"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="132"/>
+      <c r="H12" s="133"/>
       <c r="K12" s="79" t="s">
         <v>7</v>
       </c>
@@ -12261,13 +12720,13 @@
       <c r="AV12" s="4"/>
     </row>
     <row r="13" spans="2:48" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="130"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="131"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="131"/>
-      <c r="H13" s="132"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="132"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="132"/>
+      <c r="H13" s="133"/>
       <c r="K13" s="58" t="s">
         <v>8</v>
       </c>
@@ -12301,13 +12760,13 @@
       <c r="AV13" s="4"/>
     </row>
     <row r="14" spans="2:48" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="130"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="131"/>
-      <c r="G14" s="131"/>
-      <c r="H14" s="132"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="133"/>
       <c r="K14" s="58" t="s">
         <v>9</v>
       </c>
@@ -12341,13 +12800,13 @@
       <c r="AV14" s="4"/>
     </row>
     <row r="15" spans="2:48" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="130"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="132"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="133"/>
       <c r="K15" s="58" t="s">
         <v>10</v>
       </c>
@@ -12374,13 +12833,13 @@
       <c r="AV15" s="4"/>
     </row>
     <row r="16" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="130"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="132"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="133"/>
       <c r="K16" s="58" t="s">
         <v>11</v>
       </c>
@@ -12407,13 +12866,13 @@
       <c r="AV16" s="4"/>
     </row>
     <row r="17" spans="2:48" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="130"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="132"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="132"/>
+      <c r="H17" s="133"/>
       <c r="K17" s="58" t="s">
         <v>12</v>
       </c>
@@ -12440,13 +12899,13 @@
       <c r="AV17" s="4"/>
     </row>
     <row r="18" spans="2:48" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="133"/>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="135"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="136"/>
       <c r="K18" s="58" t="s">
         <v>13</v>
       </c>
@@ -12495,15 +12954,15 @@
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="2:48" ht="25.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
-      <c r="H20" s="126"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20" s="58" t="s">
@@ -12792,15 +13251,15 @@
       <c r="AV29" s="4"/>
     </row>
     <row r="30" spans="2:48" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="126" t="s">
+      <c r="B30" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="126"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="126"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="126"/>
-      <c r="H30" s="126"/>
+      <c r="C30" s="127"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
+      <c r="F30" s="127"/>
+      <c r="G30" s="127"/>
+      <c r="H30" s="127"/>
       <c r="I30" s="45"/>
       <c r="J30" s="45"/>
       <c r="K30" s="58" t="s">
@@ -13074,14 +13533,14 @@
       <c r="E41" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="G41" s="123" t="s">
+      <c r="G41" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="H41" s="124"/>
-      <c r="I41" s="124"/>
-      <c r="J41" s="124"/>
-      <c r="K41" s="124"/>
-      <c r="L41" s="125"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="125"/>
+      <c r="J41" s="125"/>
+      <c r="K41" s="125"/>
+      <c r="L41" s="126"/>
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
@@ -13116,14 +13575,14 @@
         <v>15</v>
       </c>
       <c r="F42" s="37"/>
-      <c r="G42" s="139" t="s">
+      <c r="G42" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="H42" s="140"/>
-      <c r="I42" s="140"/>
-      <c r="J42" s="140"/>
-      <c r="K42" s="140"/>
-      <c r="L42" s="141"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
+      <c r="J42" s="141"/>
+      <c r="K42" s="141"/>
+      <c r="L42" s="142"/>
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
@@ -13158,14 +13617,14 @@
         <v>12</v>
       </c>
       <c r="F43" s="37"/>
-      <c r="G43" s="142" t="s">
+      <c r="G43" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="H43" s="143"/>
-      <c r="I43" s="143"/>
-      <c r="J43" s="143"/>
-      <c r="K43" s="143"/>
-      <c r="L43" s="144"/>
+      <c r="H43" s="144"/>
+      <c r="I43" s="144"/>
+      <c r="J43" s="144"/>
+      <c r="K43" s="144"/>
+      <c r="L43" s="145"/>
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
       <c r="AF43" s="4"/>
@@ -13200,14 +13659,14 @@
         <v>31</v>
       </c>
       <c r="F44" s="37"/>
-      <c r="G44" s="120" t="s">
+      <c r="G44" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121"/>
-      <c r="J44" s="121"/>
-      <c r="K44" s="121"/>
-      <c r="L44" s="122"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="122"/>
+      <c r="J44" s="122"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="123"/>
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
       <c r="AF44" s="4"/>

</xml_diff>